<commit_message>
collapse so that only one unique courses
</commit_message>
<xml_diff>
--- a/outs/MK8WR_rmkd.xlsx
+++ b/outs/MK8WR_rmkd.xlsx
@@ -149,10 +149,10 @@
     <t xml:space="preserve">GCN Sherbet Land</t>
   </si>
   <si>
+    <t xml:space="preserve">Thwomp Ruins</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tour Paris Promenade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thwomp Ruins</t>
   </si>
   <si>
     <t xml:space="preserve">Bone-Dry Dunes</t>
@@ -642,13 +642,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.531425995577844</v>
+        <v>0.537462078211016</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>265.712997788922</v>
+        <v>268.731039105508</v>
       </c>
     </row>
     <row r="5">
@@ -740,13 +740,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.580091968781694</v>
+        <v>0.570796331225673</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>290.045984390847</v>
+        <v>285.398165612837</v>
       </c>
     </row>
     <row r="12">
@@ -824,13 +824,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.598194767182003</v>
+        <v>0.5973397048452</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>299.097383591001</v>
+        <v>298.6698524226</v>
       </c>
     </row>
     <row r="18">
@@ -936,13 +936,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="n">
-        <v>0.685341177246376</v>
+        <v>0.685250221723626</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>342.670588623188</v>
+        <v>342.625110861813</v>
       </c>
     </row>
     <row r="26">
@@ -992,13 +992,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="n">
-        <v>0.694001572774329</v>
+        <v>0.693760190810109</v>
       </c>
       <c r="C29" t="n">
         <v>28</v>
       </c>
       <c r="D29" t="n">
-        <v>347.000786387164</v>
+        <v>346.880095405054</v>
       </c>
     </row>
     <row r="30">
@@ -1188,13 +1188,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="n">
-        <v>0.734535215055572</v>
+        <v>0.72759375775852</v>
       </c>
       <c r="C43" t="n">
         <v>42</v>
       </c>
       <c r="D43" t="n">
-        <v>367.267607527786</v>
+        <v>363.79687887926</v>
       </c>
     </row>
     <row r="44">
@@ -1202,13 +1202,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="n">
-        <v>0.737655320618927</v>
+        <v>0.734535215055572</v>
       </c>
       <c r="C44" t="n">
         <v>43</v>
       </c>
       <c r="D44" t="n">
-        <v>368.827660309464</v>
+        <v>367.267607527786</v>
       </c>
     </row>
     <row r="45">
@@ -1706,13 +1706,13 @@
         <v>82</v>
       </c>
       <c r="B80" t="n">
-        <v>0.974191732072298</v>
+        <v>0.974679049688625</v>
       </c>
       <c r="C80" t="n">
         <v>79</v>
       </c>
       <c r="D80" t="n">
-        <v>487.095866036149</v>
+        <v>487.339524844312</v>
       </c>
     </row>
     <row r="81">

</xml_diff>

<commit_message>
run with updated etl data
</commit_message>
<xml_diff>
--- a/outs/MK8WR_rmkd.xlsx
+++ b/outs/MK8WR_rmkd.xlsx
@@ -936,13 +936,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="n">
-        <v>0.685250221723626</v>
+        <v>0.684641519379073</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>342.625110861813</v>
+        <v>342.320759689536</v>
       </c>
     </row>
     <row r="26">
@@ -1300,13 +1300,13 @@
         <v>53</v>
       </c>
       <c r="B51" t="n">
-        <v>0.759513958152195</v>
+        <v>0.759457985522811</v>
       </c>
       <c r="C51" t="n">
         <v>50</v>
       </c>
       <c r="D51" t="n">
-        <v>379.756979076098</v>
+        <v>379.728992761406</v>
       </c>
     </row>
     <row r="52">
@@ -1510,13 +1510,13 @@
         <v>68</v>
       </c>
       <c r="B66" t="n">
-        <v>0.806960667242508</v>
+        <v>0.805988142806957</v>
       </c>
       <c r="C66" t="n">
         <v>65</v>
       </c>
       <c r="D66" t="n">
-        <v>403.480333621254</v>
+        <v>402.994071403479</v>
       </c>
     </row>
     <row r="67">

</xml_diff>